<commit_message>
Detour Analysis for Reviewers
</commit_message>
<xml_diff>
--- a/Data/Study_01/Raw/Unique_Events_Pilot_Final.xlsx
+++ b/Data/Study_01/Raw/Unique_Events_Pilot_Final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wjpmi\Dropbox\PC (2)\Documents\GitHub\fright_night_study\Data\Study_01\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6BED0B-3CFD-4623-B0A2-9D49167DB4BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F75A5FAF-6FD7-4434-B2EF-BA1D0908D717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19080" yWindow="2115" windowWidth="19080" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27225" yWindow="4455" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -251,9 +251,6 @@
     <t>there was a man typing on a type writer when you firs enter.</t>
   </si>
   <si>
-    <t>Marissa</t>
-  </si>
-  <si>
     <t>The fact that this is when they registered that they are in a haunted house makes me think it's the first room. Also, the loud noise makes me think of the banging on the bars of the jail cells</t>
   </si>
   <si>
@@ -317,9 +314,6 @@
     <t>Final Conclusion</t>
   </si>
   <si>
-    <t>Katie</t>
-  </si>
-  <si>
     <t>Banging on something may be more consistant w/ crypt since it was first and they banged on jail cells…</t>
   </si>
   <si>
@@ -327,6 +321,12 @@
   </si>
   <si>
     <t>Could also be the meat freezer in the crypt…</t>
+  </si>
+  <si>
+    <t>Reviewer1</t>
+  </si>
+  <si>
+    <t>Reviewer2</t>
   </si>
 </sst>
 </file>
@@ -667,8 +667,8 @@
   <dimension ref="A1:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -699,19 +699,19 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="75.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -731,13 +731,13 @@
         <v>11</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I2" s="3" t="str">
         <f t="shared" ref="I2:I24" si="0">IF(E2=G2,E2,"")</f>
@@ -765,7 +765,7 @@
         <v>11</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I3" s="3" t="str">
         <f t="shared" si="0"/>
@@ -793,7 +793,7 @@
         <v>15</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I4" s="3" t="str">
         <f t="shared" si="0"/>
@@ -821,7 +821,7 @@
         <v>15</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I5" s="3" t="str">
         <f t="shared" si="0"/>
@@ -849,7 +849,7 @@
         <v>11</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I6" s="3" t="str">
         <f t="shared" si="0"/>
@@ -877,7 +877,7 @@
         <v>11</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I7" s="3" t="str">
         <f t="shared" si="0"/>
@@ -905,7 +905,7 @@
         <v>11</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -933,7 +933,7 @@
         <v>31</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I9" s="3" t="str">
         <f t="shared" si="0"/>
@@ -961,7 +961,7 @@
         <v>15</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I10" s="10" t="s">
         <v>11</v>
@@ -984,13 +984,13 @@
         <v>11</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I11" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1018,7 +1018,7 @@
         <v>7</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I12" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1046,7 +1046,7 @@
         <v>15</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I13" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1074,7 +1074,7 @@
         <v>15</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I14" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1102,7 +1102,7 @@
         <v>15</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I15" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1126,13 +1126,13 @@
         <v>15</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I16" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1159,7 +1159,7 @@
         <v>15</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I17" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1186,7 +1186,7 @@
         <v>15</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I18" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1213,7 +1213,7 @@
         <v>31</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I19" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1240,7 +1240,7 @@
         <v>15</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I20" s="10" t="s">
         <v>11</v>
@@ -1266,7 +1266,7 @@
         <v>7</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I21" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1293,7 +1293,7 @@
         <v>15</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I22" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1320,7 +1320,7 @@
         <v>15</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I23" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1347,7 +1347,7 @@
         <v>31</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I24" s="3" t="str">
         <f t="shared" si="0"/>

</xml_diff>